<commit_message>
bug fixes and added more keywords
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/hs/keyword/scenarios/hubspot_scenarios.xlsx
+++ b/src/main/java/com/qa/hs/keyword/scenarios/hubspot_scenarios.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="19300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="2" r:id="rId1"/>
-    <sheet name="login1" sheetId="1" r:id="rId2"/>
+    <sheet name="signup" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="24">
-  <si>
-    <t>locator</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
   <si>
     <t>action</t>
   </si>
@@ -39,21 +36,12 @@
     <t>value</t>
   </si>
   <si>
-    <t>id=username</t>
-  </si>
-  <si>
     <t>sendkeys</t>
   </si>
   <si>
-    <t>id=password</t>
-  </si>
-  <si>
     <t>Test@1234</t>
   </si>
   <si>
-    <t>id=loginBtn</t>
-  </si>
-  <si>
     <t>click</t>
   </si>
   <si>
@@ -84,9 +72,6 @@
     <t>open browser</t>
   </si>
   <si>
-    <t>chrome</t>
-  </si>
-  <si>
     <t>launch url</t>
   </si>
   <si>
@@ -99,14 +84,65 @@
     <t>verify sign up link</t>
   </si>
   <si>
-    <t>linkText=Sign up</t>
+    <t>locatorType</t>
+  </si>
+  <si>
+    <t>locatorValue</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>loginBtn</t>
+  </si>
+  <si>
+    <t>Sign up</t>
+  </si>
+  <si>
+    <t>linkText</t>
+  </si>
+  <si>
+    <t>verify home page header</t>
+  </si>
+  <si>
+    <t>get home page header text</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>//h1[text()='Sales Dashboard']</t>
+  </si>
+  <si>
+    <t>isDisplayed</t>
+  </si>
+  <si>
+    <t>className</t>
+  </si>
+  <si>
+    <t>private-page__title</t>
+  </si>
+  <si>
+    <t>getText</t>
+  </si>
+  <si>
+    <t>Sales Dashboard</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -130,8 +166,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,6 +203,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -154,19 +219,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -443,179 +514,178 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
+      <c r="E9" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D9" r:id="rId3"/>
+    <hyperlink ref="E4" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -623,10 +693,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD7"/>
+    <sheetView zoomScale="183" zoomScaleNormal="183" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -637,108 +707,94 @@
     <col min="4" max="4" width="27.5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
+      <c r="E5" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>